<commit_message>
Updating season ratings files for NFL, NBA and WNBA with the players who played in those seasons
</commit_message>
<xml_diff>
--- a/docs/Madden NFL/College Football/NCAA Football 06 Ratings.xlsx
+++ b/docs/Madden NFL/College Football/NCAA Football 06 Ratings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30af24b3fe5d560e/Documentos/André/Games/Documents/Sports Games/Madden NFL/College Football/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42064" documentId="11_AD4DF034E34935FBC521DCD7BFD97F025BDEDD8C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61C5574D-616D-411A-8A41-3080B839D356}"/>
+  <xr:revisionPtr revIDLastSave="42083" documentId="11_AD4DF034E34935FBC521DCD7BFD97F025BDEDD8C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4D37B7C-92A0-4F1C-938B-0890EB10DB89}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="420" windowWidth="22956" windowHeight="10440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="156" yWindow="384" windowWidth="22884" windowHeight="10476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" r:id="rId1"/>
@@ -861,7 +861,18 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor auto="1"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
@@ -883,18 +894,7 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
@@ -926,7 +926,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EFE01862-7712-4B95-AB17-44312383458C}" name="Tabela1" displayName="Tabela1" ref="A1:G2" insertRow="1" totalsRowShown="0" dataDxfId="24">
   <autoFilter ref="A1:G2" xr:uid="{EFE01862-7712-4B95-AB17-44312383458C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G2">
-    <sortCondition descending="1" ref="B1:B2"/>
+    <sortCondition ref="A1:A2"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{45DD2C62-7C3E-42FD-99E1-1C11CC08F3BC}" name="Player" dataDxfId="23"/>
@@ -1272,8 +1272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1333,7 +1333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91B5C15-9235-4990-AD10-9915F8885DD9}">
   <dimension ref="A1:F120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+    <sheetView topLeftCell="A115" workbookViewId="0">
       <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>

</xml_diff>